<commit_message>
Azriely and Sons project done
</commit_message>
<xml_diff>
--- a/training_schedule.xlsx
+++ b/training_schedule.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\CV_training\CV_training\CV_training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hadar\PycharmProjects\CV_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C7565F-996E-409F-9951-8C1C3311C435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="4220"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -123,23 +135,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,18 +457,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -470,13 +489,13 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <f>SUM(C3)</f>
         <v>0.5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>SUM(D3)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -486,18 +505,21 @@
       <c r="C3">
         <v>0.5</v>
       </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <f>SUM(C6:C11)</f>
         <v>15.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f>SUM(D6:D11)</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -507,6 +529,9 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -515,6 +540,9 @@
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -523,6 +551,9 @@
       <c r="C8">
         <v>6.5</v>
       </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -531,6 +562,9 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -539,6 +573,9 @@
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -547,31 +584,26 @@
       <c r="C11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="D11">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
-        <f>SUM(C13:C20)</f>
+      <c r="C13" s="2">
+        <f>SUM(C14:C21)</f>
         <v>13</v>
       </c>
-      <c r="D12">
-        <f>SUM(D13:D20)</f>
+      <c r="D13" s="2">
+        <f>SUM(D14:D21)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -579,7 +611,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -587,15 +619,15 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -603,7 +635,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -611,7 +643,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -619,106 +651,114 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="C21">
-        <f>SUM(C22:C24)</f>
+      <c r="C23" s="2">
+        <f>SUM(C24:C26)</f>
         <v>21</v>
       </c>
-      <c r="D21">
-        <f>SUM(D22:D24)</f>
+      <c r="D23" s="2">
+        <f>SUM(D24:D26)</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>27</v>
+      <c r="B25" t="s">
+        <v>25</v>
       </c>
       <c r="C25">
-        <f>SUM(C26:C28)</f>
-        <v>28</v>
-      </c>
-      <c r="D25">
-        <f>SUM(D26:D28)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2">
+        <f>SUM(C29:C31)</f>
+        <v>28</v>
+      </c>
+      <c r="D28" s="2">
+        <f>SUM(D29:D31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C29">
         <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f>SUM(C30:C31)</f>
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <f>SUM(D30:D31)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <f>SUM(C34:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <f>SUM(D34:D35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>